<commit_message>
Adds iTinExportEngine sample01 (banner)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c06f2c4b-6ad9-40df-bbf6-3ec16a7acc65}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f0b7016c-5a49-4213-8b58-cc57005e587b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c507921e-2c4f-411b-a584-b271070ce720}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{57030b5d-ef42-4b27-b2f9-45ff76508cf6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{24ecb1e2-2dd3-4aeb-917d-4ff63df6635d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a61764ea-57a5-4aa9-b3e4-d61a144d6e06}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fcea0272-3d85-415d-9ac1-292329e48a0d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cfe887ff-8eea-4ceb-9a0a-f19fa40beee1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6472fa7e-32d7-422d-b1b7-fdb374ba478b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6d1d9778-1197-40fb-99e7-9322251678a1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{45b82145-4db1-43f3-974e-9ae758028aab}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0015c1eb-d413-40aa-b6a0-a1afb33ed86d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c7c7e214-7835-4d24-8154-3b9c1ef4dc0e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4b8f7f9f-fb1c-4ea1-aa1b-a277f9649183}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{37cd15af-0819-45a3-b91e-067f5f3a017e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4ffff1ba-bae2-496a-957d-f988bf4a9e74}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{443f17ad-1400-4e12-a4ac-2aa8ce10a799}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{db813acc-9d82-4f3e-b786-e7956927fcee}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{498b2080-440d-4dde-9fbb-feb4ee720a12}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3e35f076-9315-487c-94c0-af93bd0d8aae}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{683771f1-1f07-4bc5-b58c-45540fc6fc46}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1c608eca-2f86-41bf-89de-3de2f306f407}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{92c80eb4-5ad4-4e51-9b29-37cd2906c3c9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{dfb29b79-093f-4dab-b1a7-14c6a597abfd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{973b676b-96d2-4fdc-8f52-d35d545d7a51}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e6789eda-3d7d-4df6-a2b6-d967fff7277c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{58a42e44-3fb2-4127-93d8-4c8dab572b84}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f95ab944-ed70-4e18-944a-f6c810c628fb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5c74d997-877c-4830-8182-04f21ff9db8d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f8f39654-6eaf-4fe4-bf86-072b0173cb9d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{698b8ca9-172e-41ba-b720-c6f2a065d88c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{91a842c6-bdfd-4635-bc5b-016344a997ba}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c30b8241-b3d1-4f14-bcf0-180225a2d556}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{51e01b4e-1ef2-46a8-97a2-92c134c1da01}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e3c72e96-e8a7-4851-b6f0-9321dea9b341}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{93d9a05c-fc08-43dd-81b0-57fe32337d9d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f75f17d5-fa51-428f-83ec-4c4c597d7499}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b56395d5-da07-4921-bc86-9db4c006fc60}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{54633958-2a34-4e95-80b8-abcfae9da694}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{16ca29b4-1c5e-4c8d-a869-7eaa00f8f43e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{370c84b7-4ec0-4c00-9808-1aa79ba1c04d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ba220fd9-8e69-4363-9328-8f22a7b75b09}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{08d2efb6-939c-49b2-aa83-abc330d3007a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e3c28046-10d9-4beb-90f8-32c607f12113}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{03c7ad69-474c-4470-a61e-f8bbd2aaac5e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7e41c5a-0c83-4b36-aaaa-ae97b9bdd9af}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b290e19c-05e7-48b6-b5f0-db99699b2f56}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{407df60b-f1e6-459e-9f39-9a599cb4cee9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{acee213e-463d-415f-8be3-47e3abe3aab9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b1144ce0-9656-490d-80cf-19453e034977}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6ec072a5-5ec4-4ece-9190-bade554e65d2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a33d76bc-cac4-431a-8fd5-7d3c72a65a04}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{abd2479b-1f17-4092-b1e5-a5c93c3941ea}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ae9b0e40-1ed1-4e26-8490-265160243fca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4d6f3f9f-80e0-4206-a30e-ca17f0dfd4a3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{617caaa3-955a-4385-a7b1-1e78fe156711}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d30e37c5-567d-482c-a300-63e49579ed06}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f795c85e-446f-404e-b22e-3037e93dcd66}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d69fbf40-08d0-4689-a112-f4a740cbef60}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b06db69b-1fc2-4b5e-931d-9961d9f022a6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{40ed0afe-eb33-48d2-901b-e03834d8b393}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{95db822d-8dee-4b62-a0bd-1f1c3db6ef5a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{706fe49f-c28f-4f50-9a24-f7e2059e260d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7dc413d6-a589-4d3d-bd15-702d0743f0e7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Adds new samples for iExportEngine in iTinExportEngineSamples
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bfe6173e-9709-4dc8-8b92-237da5f1ff96}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bd306ee4-9fbf-4b6b-8c6b-c202b8418480}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{db2a41c5-3835-4684-b516-eb0bf4fc77b7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d23d53b7-44d5-4de9-a9e2-4324eb24c95b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3649dc97-066a-4ac7-802c-0067d8bca8ed}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cfa3b69c-5df1-4763-82da-1aa844d36741}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{39188c81-8e9b-4a7d-93d0-36b83a36cbe0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1687ded7-d94b-44b1-9241-8e4796bfe933}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{291fc2da-d559-4b41-8371-2df876e42b34}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3b4e6541-6314-413c-92f0-37fa0f8eecd2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{33c1f2e3-afa7-4981-9790-d84662c040e8}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0415dbdc-ec9f-4ff0-868d-056bffb2fe25}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{acb5cdc8-3c57-49df-984e-d21cf9aff345}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e0ce1d29-4798-4391-8241-bf1e07b91362}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{23a5df75-760e-4f89-8daa-d86198a7d956}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4909a7a3-392b-4fd2-8c12-4b3fc9b57e87}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b032d235-a217-4c61-903e-f858733183ae}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{39e0dde2-8332-4ced-9c64-cf403803b6bf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1ee6d3b9-7261-4cfd-a100-4c017258ef4a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b2a84baf-025a-4db8-b2d1-316398eca831}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9d9bfbe5-1cef-42c1-b366-8ceb0238769e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f80db8da-33d5-41cc-b34f-70ca293ef01d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fb72000c-4ecc-4a00-961c-5671a4c9357c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{85d0082a-220c-4223-b16b-237653402ceb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bedc9a39-3b80-4659-a40d-4c5a9ec0a266}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{516a498e-ce2a-4cb5-bf1e-d2374c63be9b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c8068718-7899-4c70-a02f-67d5a53dd3f7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{21d10cbb-b56f-4808-8b04-b4cde3533916}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2a9989df-bba7-4cec-8716-ae71e0772303}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8e9e2e91-fb29-40b8-bb42-2f31a094dfab}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fd0a3f26-edc4-4779-b2a8-57c4147e3183}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9b4d1e85-78f4-485d-af92-f380748ad3b4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{08c186a6-48e6-4214-a53b-7a8a05867fe2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{256dcff9-3fc5-4d2c-b84e-8ca07671a6b9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a75df81e-d4d3-432e-bae3-5d8e0bfde407}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bd3ea20e-6bdc-4705-8e47-355941e6bde0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{16733ee0-ba17-4af3-8961-9c6209522a59}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b7b0c22d-2e49-4d43-837b-b95d336264e0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cb27a3f2-8f6b-4aee-addc-a151512aaa3d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6667f57d-daa0-4d73-8afc-e8850dc352a6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8a7d3c86-c164-4c56-abe0-33a22b549819}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{85345a05-a310-4f4e-a552-1c54ce392dd1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{68641314-c61a-40cc-8e91-97defde811af}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{35c2ba95-e126-4543-b355-a0296a592e7b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{417b26e3-5748-45be-b4c6-a7416035e007}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d7048f65-697b-4bee-b9f7-5b7d1a04b322}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{585c34b4-a829-4e57-a95d-9a1428709f39}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c539d0cb-6a93-451a-846a-27d9c10f0f30}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a4bdc756-836e-494c-bbc8-a0ad5130c2f6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{eac90879-594b-4e5b-990b-7cbdd593ab75}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fd9b7f13-ac64-470d-b8eb-82dc5a7a9539}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{06741fd1-1556-4c1b-a49d-a78d85352639}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bc274f2f-fc41-42e3-9ed7-623b43b14387}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{26f55c66-4e11-4120-9ea0-c33aadc00367}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{81f4433a-f9d3-4df6-92dd-b57fc0204f2a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{18bb45c2-6419-445b-a410-28819a7a34d3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{54acab6d-19ef-4440-a865-dfc7f91114c9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{87b79f76-bc49-4efb-87eb-89f021fa2963}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d9c4f472-d5d9-4e75-bc84-71fbf47ec69b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b92472a6-392d-445a-b7e9-8d3313d3d08d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aa4e0fc5-f54f-4fd7-baf7-5e50c3838c91}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{74991e35-714e-4f68-81ef-02562859ddba}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{76cfbcd9-1949-4335-8652-c3da1cfcec40}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9dca3233-a345-43e3-b204-d206174007ec}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>